<commit_message>
excel to object array in main method
</commit_message>
<xml_diff>
--- a/test_data/open_emr_test_data.xlsx
+++ b/test_data/open_emr_test_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balaji\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mine\Company\JohnDeere\selenium_workspace\OpenEMRAutomation\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
   <si>
     <t>Username</t>
   </si>
@@ -58,6 +58,21 @@
   </si>
   <si>
     <t>peter123</t>
+  </si>
+  <si>
+    <t>peter124</t>
+  </si>
+  <si>
+    <t>peter125</t>
+  </si>
+  <si>
+    <t>peter126</t>
+  </si>
+  <si>
+    <t>peter127</t>
+  </si>
+  <si>
+    <t>peter128</t>
   </si>
 </sst>
 </file>
@@ -375,15 +390,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -425,6 +443,76 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
invalid credential - dataprovider and excel
</commit_message>
<xml_diff>
--- a/test_data/open_emr_test_data.xlsx
+++ b/test_data/open_emr_test_data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Username</t>
   </si>
@@ -58,21 +58,6 @@
   </si>
   <si>
     <t>peter123</t>
-  </si>
-  <si>
-    <t>peter124</t>
-  </si>
-  <si>
-    <t>peter125</t>
-  </si>
-  <si>
-    <t>peter126</t>
-  </si>
-  <si>
-    <t>peter127</t>
-  </si>
-  <si>
-    <t>peter128</t>
   </si>
 </sst>
 </file>
@@ -390,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,76 +431,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
valid credential - connected with excel
</commit_message>
<xml_diff>
--- a/test_data/open_emr_test_data.xlsx
+++ b/test_data/open_emr_test_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="invalidCredentialTest" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>Username</t>
   </si>
@@ -58,6 +58,21 @@
   </si>
   <si>
     <t>peter123</t>
+  </si>
+  <si>
+    <t>Expected Value</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>OpenEMR</t>
+  </si>
+  <si>
+    <t>accountant</t>
   </si>
 </sst>
 </file>
@@ -377,8 +392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,14 +453,63 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
testng xml - control project and parameterization
</commit_message>
<xml_diff>
--- a/test_data/open_emr_test_data.xlsx
+++ b/test_data/open_emr_test_data.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="invalidCredentialTest" sheetId="1" r:id="rId1"/>
     <sheet name="validCredentialTest" sheetId="2" r:id="rId2"/>
+    <sheet name="addPaitentTest" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>Username</t>
   </si>
@@ -73,6 +74,33 @@
   </si>
   <si>
     <t>accountant</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Wick</t>
+  </si>
+  <si>
+    <t>2022-05-18</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Medical Record Dashboard - john wick</t>
   </si>
 </sst>
 </file>
@@ -108,8 +136,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,4 +541,82 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
extent report added with logs
</commit_message>
<xml_diff>
--- a/test_data/open_emr_test_data.xlsx
+++ b/test_data/open_emr_test_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="invalidCredentialTest" sheetId="1" r:id="rId1"/>
@@ -490,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +538,7 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
@@ -553,7 +553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
page object added - non-static
</commit_message>
<xml_diff>
--- a/test_data/open_emr_test_data.xlsx
+++ b/test_data/open_emr_test_data.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>Username</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>OpenEMR</t>
-  </si>
-  <si>
-    <t>accountant</t>
   </si>
   <si>
     <t>FirstName</t>
@@ -488,10 +485,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C3"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,20 +524,6 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -581,19 +564,19 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" t="s">
-        <v>19</v>
-      </c>
       <c r="H1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I1" t="s">
         <v>11</v>
@@ -610,22 +593,22 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" t="s">
-        <v>23</v>
-      </c>
       <c r="H2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>